<commit_message>
write test results to r3 excel file changes are added
</commit_message>
<xml_diff>
--- a/src/test/testdata/Accurate_Bucket_ORG_PROV_Phone.xlsx
+++ b/src/test/testdata/Accurate_Bucket_ORG_PROV_Phone.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R3_Test_Automation\R3_Test_Automation\src\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6419A3DE-3BDA-4FFF-B853-68A38D90BE29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D347271A-4EF3-41FF-8D6A-4B8C2A32FA82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2855E3E2-C5F0-4EF0-BC43-ED693B49271B}"/>
   </bookViews>
@@ -83,7 +83,7 @@
     <t>No. of R3 Excel Row's to Execute</t>
   </si>
   <si>
-    <t>200</t>
+    <t>100</t>
   </si>
 </sst>
 </file>
@@ -488,7 +488,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
1.1 code 4, 5 points are pending
</commit_message>
<xml_diff>
--- a/src/test/testdata/Accurate_Bucket_ORG_PROV_Phone.xlsx
+++ b/src/test/testdata/Accurate_Bucket_ORG_PROV_Phone.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R3_Test_Automation\R3_Test_Automation\src\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D347271A-4EF3-41FF-8D6A-4B8C2A32FA82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D85825-77B3-42FA-82AD-117AF79EBE93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2855E3E2-C5F0-4EF0-BC43-ED693B49271B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2855E3E2-C5F0-4EF0-BC43-ED693B49271B}"/>
   </bookViews>
   <sheets>
     <sheet name="ORG_PROV_Phone_Scenario" sheetId="1" r:id="rId1"/>
@@ -83,7 +83,7 @@
     <t>No. of R3 Excel Row's to Execute</t>
   </si>
   <si>
-    <t>100</t>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -488,22 +488,22 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.7109375" style="5" customWidth="1"/>
-    <col min="4" max="5" width="34.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="31.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.7265625" style="5" customWidth="1"/>
+    <col min="4" max="5" width="34.54296875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -529,7 +529,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>

</xml_diff>